<commit_message>
finished data merger and data collector
</commit_message>
<xml_diff>
--- a/static_data/measures/measures.xlsx
+++ b/static_data/measures/measures.xlsx
@@ -379,7 +379,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -424,15 +424,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD37"/>
+  <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="S1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.5"/>
@@ -452,6 +452,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="24.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="15.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="15.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1015" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="61" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -524,15 +525,8 @@
       <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>23</v>
       </c>
@@ -602,15 +596,8 @@
       <c r="W2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>34</v>
       </c>
@@ -680,13 +667,6 @@
       <c r="W3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="147" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
@@ -750,15 +730,8 @@
       <c r="W4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>61</v>
       </c>
@@ -805,15 +778,8 @@
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>67</v>
       </c>
@@ -846,15 +812,8 @@
       <c r="R6" s="3"/>
       <c r="U6" s="3"/>
       <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>73</v>
       </c>
@@ -882,15 +841,8 @@
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>43831</v>
       </c>
@@ -960,15 +912,8 @@
       <c r="W8" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>43889</v>
       </c>
@@ -976,7 +921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>43901</v>
       </c>
@@ -984,7 +929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
         <v>43903</v>
       </c>
@@ -1010,7 +955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
         <v>43906</v>
       </c>
@@ -1051,7 +996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
         <v>43910</v>
       </c>
@@ -1059,7 +1004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
         <v>43948</v>
       </c>
@@ -1067,7 +1012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
         <v>43962</v>
       </c>
@@ -1096,7 +1041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
         <v>43979</v>
       </c>
@@ -1104,12 +1049,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
         <v>43983</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
         <v>43988</v>
       </c>
@@ -1138,7 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
         <v>43997</v>
       </c>
@@ -1146,7 +1091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
         <v>44002</v>
       </c>
@@ -1157,7 +1102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="n">
         <v>44004</v>
       </c>
@@ -1180,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="n">
         <v>44018</v>
       </c>
@@ -1188,12 +1133,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="n">
         <v>44058</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="n">
         <v>44105</v>
       </c>
@@ -1201,7 +1146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="n">
         <v>44123</v>
       </c>
@@ -1221,7 +1166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="n">
         <v>44132</v>
       </c>
@@ -1241,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="n">
         <v>44174</v>
       </c>
@@ -1253,7 +1198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="n">
         <v>44177</v>
       </c>
@@ -1264,7 +1209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="n">
         <v>44186</v>
       </c>
@@ -1272,7 +1217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="n">
         <v>44187</v>
       </c>
@@ -1286,7 +1231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="n">
         <v>44193</v>
       </c>
@@ -1297,12 +1242,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="n">
         <v>44205</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="n">
         <v>44214</v>
       </c>
@@ -1319,7 +1264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="n">
         <v>44228</v>
       </c>
@@ -1327,17 +1272,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="n">
         <v>44235</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="n">
         <v>44224</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="n">
         <v>44256</v>
       </c>
@@ -1376,7 +1321,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.83"/>
   </cols>
@@ -1462,7 +1407,7 @@
       <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1600,7 +1545,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1714,7 +1659,7 @@
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1820,7 +1765,7 @@
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1902,7 +1847,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1961,7 +1906,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2023,7 +1968,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2069,7 +2014,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2142,7 +2087,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2220,7 +2165,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2268,7 +2213,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.33"/>
   </cols>
@@ -2384,7 +2329,7 @@
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2431,7 +2376,7 @@
       <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.5"/>
   </cols>
@@ -2628,7 +2573,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2681,7 +2626,7 @@
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.5"/>
@@ -2809,7 +2754,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2933,7 +2878,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
   </cols>
@@ -3078,7 +3023,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3137,7 +3082,7 @@
       <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3185,7 +3130,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
   </cols>
@@ -3275,7 +3220,7 @@
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.66"/>
   </cols>
@@ -3398,7 +3343,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.83"/>
   </cols>
@@ -3503,7 +3448,7 @@
       <selection pane="topLeft" activeCell="J44" activeCellId="0" sqref="J44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3576,7 +3521,7 @@
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3689,7 +3634,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
trained some simple ML models
</commit_message>
<xml_diff>
--- a/static_data/measures/measures.xlsx
+++ b/static_data/measures/measures.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="77">
   <si>
     <t xml:space="preserve">Time</t>
   </si>
@@ -69,211 +69,214 @@
     <t xml:space="preserve">Upper secondary school, vocational schools and higher education</t>
   </si>
   <si>
+    <t xml:space="preserve">universities and other educational establishments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mountain railways</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homeworking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restaurants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discos/Nightclubs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shops/Markets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penalties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mask mandatory in publicly accessible establishments/ spaces (shops etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mask mandatory in public transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masks mandatory in schools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masks mandatory at work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cultural, entertainment and recreational facilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sport/Wellness facilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sport activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Religious services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Singing allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 0 (default at start)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open with no restrictions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no people limit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">no restrictions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no people limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">as usual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no penalties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no restrictions (with physical contact)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open with some restrictions (quarantine from risk area, PCR test, contact data)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ban for events with more than 1000 people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restrictions at private events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no people limit but wear a mask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open with protection concept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recommendation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open with protection concept (including capacity restriction)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">penalties based only on epedemic law (e.g. quarantine or isolation violation, business does not close, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sport activities possible with no physical contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ban for professionals and amateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Border closed to at least one none direct border sharing country </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ban for events with more than 300 people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ban for gatherings with more than 30 people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ban for demonstrations with more than 1000 people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closed but exams are possible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compulsory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open with protection concept and other restrictions (time, max people, max group size, seated consumption)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open but time limitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fines are possible (e.g. gathering in large groups or not wearing masks when it is mandatory)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some at low risk categorized facilities are open (e.g. museums, libraries etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">outdoor open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sport activities only very restricted possible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closed (but some exceptions for funerals)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ban for all people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Border closed to one country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ban for events with more than 100 people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ban for gatherings with more than 15 people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ban for demonstrations with more than 300 people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some as low risk categorized shops are open (like car washes, DIY, hairdresser)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Border closed to all bordering countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ban on events with more than 50 people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ban for gatherings with more than 10 people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ban for demonstrations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closed (except day-to-day necesities)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">complete ban of events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ban for gatherings with more than 5 people</t>
+  </si>
+  <si>
     <t xml:space="preserve">universities and other educational establishments </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mountain railways</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Homeworking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restaurants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discos/Nightclubs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shops/Markets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Penalties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mask mandatory in publicly accessible establishments/ spaces (shops etc.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mask mandatory in public transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masks mandatory in schools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masks mandatory at work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cultural, entertainment and recreational facilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sport/Wellness facilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sport activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Religious services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Singing allowed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category 0 (default at start)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open with no restrictions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no people limit </t>
-  </si>
-  <si>
-    <t xml:space="preserve">no restrictions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no people limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">as usual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no penalties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no restrictions (with physical contact)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open with some restrictions (quarantine from risk area, PCR test, contact data)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ban for events with more than 1000 people</t>
-  </si>
-  <si>
-    <t xml:space="preserve">restrictions at private events</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no people limit but wear a mask</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open with protection concept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">recommendation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open with protection concept (including capacity restriction)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">penalties based only on epedemic law (e.g. quarantine or isolation violation, business does not close, etc.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sport activities possible with no physical contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ban for professionals and amateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Border closed to at least one none direct border sharing country </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ban for events with more than 300 people</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ban for gatherings with more than 30 people</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ban for demonstrations with more than 1000 people</t>
-  </si>
-  <si>
-    <t xml:space="preserve">closed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">closed but exams are possible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compulsory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open with protection concept and other restrictions (time, max people, max group size, seated consumption)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open but time limitation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fines are possible (e.g. gathering in large groups or not wearing masks when it is mandatory)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">some at low risk categorized facilities are open (e.g. museums, libraries etc.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">outdoor open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sport activities only very restricted possible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">closed (but some exceptions for funerals)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ban for all people</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Border closed to one country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ban for events with more than 100 people</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ban for gatherings with more than 15 people</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ban for demonstrations with more than 300 people</t>
-  </si>
-  <si>
-    <t xml:space="preserve">some as low risk categorized shops are open (like car washes, DIY, hairdresser)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Border closed to all bordering countries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ban on events with more than 50 people</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ban for gatherings with more than 10 people</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ban for demonstrations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">closed (except day-to-day necesities)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">complete ban of events</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ban for gatherings with more than 5 people</t>
   </si>
 </sst>
 </file>
@@ -427,12 +430,12 @@
   <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
+      <selection pane="topRight" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.5"/>
@@ -1321,7 +1324,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.83"/>
   </cols>
@@ -1407,7 +1410,7 @@
       <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1545,7 +1548,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1659,7 +1662,7 @@
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1765,7 +1768,7 @@
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1847,7 +1850,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1906,7 +1909,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1968,7 +1971,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2014,7 +2017,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2087,7 +2090,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2165,7 +2168,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2213,7 +2216,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.33"/>
   </cols>
@@ -2329,7 +2332,7 @@
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2376,7 +2379,7 @@
       <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.5"/>
   </cols>
@@ -2398,7 +2401,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -2573,7 +2576,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2626,7 +2629,7 @@
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.5"/>
@@ -2646,7 +2649,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2754,7 +2757,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2878,7 +2881,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
   </cols>
@@ -3023,7 +3026,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3082,7 +3085,7 @@
       <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3130,7 +3133,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
   </cols>
@@ -3220,7 +3223,7 @@
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.66"/>
   </cols>
@@ -3343,7 +3346,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.83"/>
   </cols>
@@ -3448,7 +3451,7 @@
       <selection pane="topLeft" activeCell="J44" activeCellId="0" sqref="J44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3521,7 +3524,7 @@
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3634,7 +3637,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
major changes in MLModel and DataPreperator
</commit_message>
<xml_diff>
--- a/static_data/measures/measures.xlsx
+++ b/static_data/measures/measures.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="76">
   <si>
     <t xml:space="preserve">Time</t>
   </si>
@@ -274,9 +274,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ban for gatherings with more than 5 people</t>
-  </si>
-  <si>
-    <t xml:space="preserve">universities and other educational establishments </t>
   </si>
 </sst>
 </file>
@@ -432,10 +429,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.5"/>
@@ -1324,7 +1321,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.83"/>
   </cols>
@@ -1410,7 +1407,7 @@
       <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1548,7 +1545,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1662,7 +1659,7 @@
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1768,7 +1765,7 @@
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1850,7 +1847,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1909,7 +1906,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1971,7 +1968,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2017,7 +2014,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2090,7 +2087,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2168,7 +2165,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2216,7 +2213,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.33"/>
   </cols>
@@ -2332,7 +2329,7 @@
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2376,15 +2373,15 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2401,7 +2398,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -2576,7 +2573,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2626,16 +2623,16 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2649,7 +2646,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2757,7 +2754,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2881,7 +2878,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
   </cols>
@@ -3026,7 +3023,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3085,7 +3082,7 @@
       <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3130,10 +3127,10 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
   </cols>
@@ -3223,7 +3220,7 @@
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.66"/>
   </cols>
@@ -3346,7 +3343,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.83"/>
   </cols>
@@ -3451,7 +3448,7 @@
       <selection pane="topLeft" activeCell="J44" activeCellId="0" sqref="J44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3524,7 +3521,7 @@
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3637,7 +3634,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
updated measures of federal council and implemented test validation and train split
</commit_message>
<xml_diff>
--- a/static_data/measures/measures.xlsx
+++ b/static_data/measures/measures.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="75">
   <si>
     <t xml:space="preserve">Time</t>
   </si>
@@ -69,7 +69,7 @@
     <t xml:space="preserve">Upper secondary school, vocational schools and higher education</t>
   </si>
   <si>
-    <t xml:space="preserve">universities and other educational establishments</t>
+    <t xml:space="preserve">Universities and other educational establishments</t>
   </si>
   <si>
     <t xml:space="preserve">Mountain railways</t>
@@ -180,13 +180,13 @@
     <t xml:space="preserve">sport activities possible with no physical contact</t>
   </si>
   <si>
-    <t xml:space="preserve">ban for professionals and amateur</t>
+    <t xml:space="preserve">ban for some people (professionals, amateur, adults)</t>
   </si>
   <si>
     <t xml:space="preserve">Category 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Border closed to at least one none direct border sharing country </t>
+    <t xml:space="preserve">Borders closed to one direct neighbor country</t>
   </si>
   <si>
     <t xml:space="preserve">ban for events with more than 300 people</t>
@@ -234,7 +234,7 @@
     <t xml:space="preserve">Category 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Border closed to one country</t>
+    <t xml:space="preserve">Borders closed to all direct neighbor countries</t>
   </si>
   <si>
     <t xml:space="preserve">ban for events with more than 100 people</t>
@@ -250,9 +250,6 @@
   </si>
   <si>
     <t xml:space="preserve">Category 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Border closed to all bordering countries</t>
   </si>
   <si>
     <t xml:space="preserve">ban on events with more than 50 people</t>
@@ -424,15 +421,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W37"/>
+  <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B5" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="topRight" activeCell="D37" activeCellId="0" sqref="D37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.5"/>
@@ -779,21 +776,18 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -803,7 +797,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -815,13 +809,13 @@
     </row>
     <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1088,7 +1082,7 @@
         <v>43997</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1213,9 +1207,6 @@
       <c r="A29" s="5" t="n">
         <v>44186</v>
       </c>
-      <c r="B29" s="0" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="n">
@@ -1235,11 +1226,8 @@
       <c r="A31" s="5" t="n">
         <v>44193</v>
       </c>
-      <c r="B31" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="H31" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1284,19 +1272,53 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="n">
+        <v>44256</v>
+      </c>
+      <c r="S37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="T37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="W37" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="n">
         <v>44277</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D38" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="M37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S37" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="T37" s="0" t="n">
-        <v>2</v>
+      <c r="M38" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="n">
+        <v>44305</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="S39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U39" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1317,16 +1339,16 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="117.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1403,11 +1425,11 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1541,11 +1563,11 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1655,11 +1677,11 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1761,11 +1783,11 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1843,11 +1865,11 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1902,11 +1924,11 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1964,11 +1986,11 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2010,11 +2032,11 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2083,11 +2105,11 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2161,11 +2183,11 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2209,11 +2231,11 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.33"/>
   </cols>
@@ -2325,11 +2347,11 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2372,11 +2394,11 @@
   </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.5"/>
   </cols>
@@ -2569,11 +2591,11 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2622,11 +2644,11 @@
   </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.5"/>
@@ -2750,11 +2772,11 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2874,16 +2896,16 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="128.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3019,11 +3041,11 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3078,11 +3100,11 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3126,16 +3148,16 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="127.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3216,11 +3238,11 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.66"/>
   </cols>
@@ -3339,11 +3361,11 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.83"/>
   </cols>
@@ -3444,11 +3466,11 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J44" activeCellId="0" sqref="J44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3517,11 +3539,11 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3630,11 +3652,11 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
updated measures (they are up to date until and with 25.6.21)
</commit_message>
<xml_diff>
--- a/static_data/measures/measures.xlsx
+++ b/static_data/measures/measures.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="74">
   <si>
     <t xml:space="preserve">Time</t>
   </si>
@@ -232,9 +232,6 @@
   </si>
   <si>
     <t xml:space="preserve">Category 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borders closed to all direct neighbor countries</t>
   </si>
   <si>
     <t xml:space="preserve">ban for events with more than 100 people</t>
@@ -421,15 +418,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W39"/>
+  <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B8" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topRight" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.5"/>
@@ -732,17 +729,17 @@
       <c r="A5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>50</v>
@@ -759,7 +756,7 @@
         <v>50</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -778,16 +775,16 @@
     </row>
     <row r="6" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -797,7 +794,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -809,13 +806,13 @@
     </row>
     <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1320,6 +1317,23 @@
       <c r="U39" s="0" t="n">
         <v>1</v>
       </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="n">
+        <v>44347</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1343,7 +1357,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.83"/>
   </cols>
@@ -1429,7 +1443,7 @@
       <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1567,7 +1581,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1681,7 +1695,7 @@
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1787,7 +1801,7 @@
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1869,7 +1883,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1928,7 +1942,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1990,7 +2004,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2036,7 +2050,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2109,7 +2123,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2187,7 +2201,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2235,7 +2249,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.33"/>
   </cols>
@@ -2351,7 +2365,7 @@
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2398,7 +2412,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.5"/>
   </cols>
@@ -2595,7 +2609,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2648,7 +2662,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.5"/>
@@ -2776,7 +2790,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2894,13 +2908,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
   </cols>
@@ -3020,6 +3034,14 @@
         <v>44214</v>
       </c>
       <c r="E11" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="n">
+        <v>44202</v>
+      </c>
+      <c r="F12" s="0" t="n">
         <v>-1</v>
       </c>
     </row>
@@ -3042,10 +3064,10 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3104,7 +3126,7 @@
       <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3152,7 +3174,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
   </cols>
@@ -3242,7 +3264,7 @@
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.66"/>
   </cols>
@@ -3362,10 +3384,10 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.83"/>
   </cols>
@@ -3470,7 +3492,7 @@
       <selection pane="topLeft" activeCell="J44" activeCellId="0" sqref="J44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3543,7 +3565,7 @@
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3656,7 +3678,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>